<commit_message>
Lots of computer software experiments
</commit_message>
<xml_diff>
--- a/Tilty Hardware/Board Files/Tilty Duo:Quad/BOM.xlsx
+++ b/Tilty Hardware/Board Files/Tilty Duo:Quad/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-38400" yWindow="-440" windowWidth="38400" windowHeight="24000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tilty Duo BT" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="133">
   <si>
     <t>Part</t>
   </si>
@@ -325,9 +325,6 @@
     <t>Check</t>
   </si>
   <si>
-    <t>Cost per 50 boards</t>
-  </si>
-  <si>
     <t xml:space="preserve">LTST-C150KGKT </t>
   </si>
   <si>
@@ -409,9 +406,6 @@
     <t>QFN/Leadless</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -419,6 +413,15 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>Prices Are based on a full population of the Tilty Quad w/ BT</t>
+  </si>
+  <si>
+    <t>Prices should drop significantly without through-hole parts</t>
+  </si>
+  <si>
+    <t>Awesomely cheap PCB manufacture (&lt;$2/board)</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -559,8 +562,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -611,8 +618,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="53">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -638,6 +652,8 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -661,6 +677,8 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -993,7 +1011,7 @@
   <dimension ref="A1:R63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1055,7 +1073,7 @@
         <v>2</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -2346,8 +2364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2409,7 +2427,7 @@
         <v>2</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -2612,22 +2630,22 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
         <v>111</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>112</v>
       </c>
       <c r="G7" s="14">
         <v>1.06</v>
@@ -2666,7 +2684,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" s="4">
         <v>0.16666666666666666</v>
@@ -2806,7 +2824,7 @@
         <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="5">
         <v>2</v>
@@ -3021,7 +3039,7 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D18" s="5">
         <v>2</v>
@@ -3254,7 +3272,12 @@
       <c r="R24" s="15"/>
     </row>
     <row r="25" spans="1:18">
-      <c r="B25" s="9"/>
+      <c r="A25" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="32">
+        <v>16</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -3265,7 +3288,12 @@
       <c r="R25" s="15"/>
     </row>
     <row r="26" spans="1:18">
-      <c r="B26" s="9"/>
+      <c r="A26" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="31">
+        <v>8</v>
+      </c>
       <c r="D26" s="5"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -3276,7 +3304,12 @@
       <c r="R26" s="15"/>
     </row>
     <row r="27" spans="1:18">
-      <c r="B27" s="9"/>
+      <c r="A27" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="31">
+        <v>8</v>
+      </c>
       <c r="D27" s="5"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -3286,7 +3319,12 @@
       <c r="O27" s="10"/>
     </row>
     <row r="28" spans="1:18">
-      <c r="B28" s="9"/>
+      <c r="A28" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="31">
+        <v>5</v>
+      </c>
       <c r="D28" s="5"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -3297,7 +3335,12 @@
       <c r="R28" s="15"/>
     </row>
     <row r="29" spans="1:18">
-      <c r="B29" s="9"/>
+      <c r="A29" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="31">
+        <v>1</v>
+      </c>
       <c r="D29" s="5"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -3603,6 +3646,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="B13:B21" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3616,7 +3662,7 @@
   <dimension ref="A1:Q63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3679,7 +3725,7 @@
         <v>2</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -3736,7 +3782,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>36</v>
@@ -3766,7 +3812,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="L3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N3" s="11"/>
       <c r="O3" s="10"/>
@@ -3953,7 +3999,7 @@
         <v>46</v>
       </c>
       <c r="M7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N7" s="17">
         <v>1.97</v>
@@ -4133,7 +4179,7 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G13" s="2">
         <v>0.37</v>
@@ -4154,7 +4200,7 @@
         <v>46</v>
       </c>
       <c r="M13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N13" s="12">
         <v>4.6899999999999997E-2</v>
@@ -4782,7 +4828,7 @@
         <v>46</v>
       </c>
       <c r="M27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N27" s="11">
         <v>2.69E-2</v>
@@ -4819,26 +4865,26 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>128</v>
+        <v>122</v>
+      </c>
+      <c r="B31" s="31">
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D33" s="5"/>
       <c r="G33" s="2"/>
@@ -4850,10 +4896,10 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D34" s="5"/>
       <c r="G34" s="2"/>
@@ -4865,10 +4911,10 @@
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D35" s="5"/>
       <c r="G35" s="2"/>
@@ -5136,7 +5182,9 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError sqref="B31 B16:B27 B32:B35" numberStoredAsText="1"/>
+    <ignoredError sqref="B16:B27 B32:B35" numberStoredAsText="1"/>
+    <ignoredError sqref="Q25 Q19 Q10 Q4" formula="1"/>
+    <ignoredError sqref="Q29" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5151,7 +5199,7 @@
   <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5214,7 +5262,7 @@
         <v>2</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -5446,7 +5494,7 @@
         <v>46</v>
       </c>
       <c r="M6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N6" s="17">
         <v>1.97</v>
@@ -5511,22 +5559,22 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
         <v>111</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>112</v>
       </c>
       <c r="G9" s="14">
         <v>1.06</v>
@@ -5566,7 +5614,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="4">
         <v>0.16666666666666666</v>
@@ -5714,7 +5762,7 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D15" s="5">
         <v>2</v>
@@ -5923,7 +5971,7 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D20" s="5">
         <v>4</v>
@@ -6210,7 +6258,7 @@
         <v>46</v>
       </c>
       <c r="M25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N25" s="11">
         <v>2.69E-2</v>
@@ -6548,10 +6596,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6561,124 +6609,130 @@
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="23">
+        <v>17.559999999999999</v>
+      </c>
+      <c r="C3" s="24">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="21" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="23">
-        <v>17.79</v>
-      </c>
-      <c r="C2" s="24">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="23">
+      <c r="B4" s="23">
         <v>30.82</v>
-      </c>
-      <c r="C3" s="24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="23">
-        <v>40.590000000000003</v>
       </c>
       <c r="C4" s="24">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:6">
       <c r="A5" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="23">
+        <v>40.590000000000003</v>
+      </c>
+      <c r="C5" s="24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="23">
+        <v>23.87</v>
+      </c>
+      <c r="C6" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="23">
-        <v>23.87</v>
-      </c>
-      <c r="C5" s="24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="25" t="s">
+      <c r="B7" s="23">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="C7" s="24">
+        <v>15</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="23">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="C6" s="24">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="23">
+      <c r="B8" s="23">
         <v>35.03</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C8" s="24">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:6">
       <c r="A9" s="21"/>
       <c r="B9" s="22"/>
       <c r="C9" s="24"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:6">
       <c r="A10" s="21"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:6">
       <c r="A11" s="21"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:6">
       <c r="A12" s="21"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:6">
       <c r="A13" s="21"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:6">
       <c r="A14" s="21"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:6">
       <c r="A15" s="21"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:6">
       <c r="A16" s="21"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24"/>

</xml_diff>